<commit_message>
delete some files database
</commit_message>
<xml_diff>
--- a/StROBe/Data/EV_load_profile.xlsx
+++ b/StROBe/Data/EV_load_profile.xlsx
@@ -5879,52 +5879,52 @@
     </row>
     <row r="1102" spans="1:1">
       <c r="A1102">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1103" spans="1:1">
       <c r="A1103">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1104" spans="1:1">
       <c r="A1104">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1105" spans="1:1">
       <c r="A1105">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1106" spans="1:1">
       <c r="A1106">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1107" spans="1:1">
       <c r="A1107">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1108" spans="1:1">
       <c r="A1108">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1109" spans="1:1">
       <c r="A1109">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1110" spans="1:1">
       <c r="A1110">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1111" spans="1:1">
       <c r="A1111">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1112" spans="1:1">
@@ -6129,952 +6129,952 @@
     </row>
     <row r="1152" spans="1:1">
       <c r="A1152">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1153" spans="1:1">
       <c r="A1153">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1154" spans="1:1">
       <c r="A1154">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1155" spans="1:1">
       <c r="A1155">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1156" spans="1:1">
       <c r="A1156">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1157" spans="1:1">
       <c r="A1157">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1158" spans="1:1">
       <c r="A1158">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1159" spans="1:1">
       <c r="A1159">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1160" spans="1:1">
       <c r="A1160">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1161" spans="1:1">
       <c r="A1161">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1162" spans="1:1">
       <c r="A1162">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1163" spans="1:1">
       <c r="A1163">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1164" spans="1:1">
       <c r="A1164">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1165" spans="1:1">
       <c r="A1165">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1166" spans="1:1">
       <c r="A1166">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1167" spans="1:1">
       <c r="A1167">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1168" spans="1:1">
       <c r="A1168">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1169" spans="1:1">
       <c r="A1169">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1170" spans="1:1">
       <c r="A1170">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1171" spans="1:1">
       <c r="A1171">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1172" spans="1:1">
       <c r="A1172">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1173" spans="1:1">
       <c r="A1173">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1174" spans="1:1">
       <c r="A1174">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1175" spans="1:1">
       <c r="A1175">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1176" spans="1:1">
       <c r="A1176">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1177" spans="1:1">
       <c r="A1177">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1178" spans="1:1">
       <c r="A1178">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1179" spans="1:1">
       <c r="A1179">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1180" spans="1:1">
       <c r="A1180">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1181" spans="1:1">
       <c r="A1181">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1182" spans="1:1">
       <c r="A1182">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1183" spans="1:1">
       <c r="A1183">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1184" spans="1:1">
       <c r="A1184">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1185" spans="1:1">
       <c r="A1185">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1186" spans="1:1">
       <c r="A1186">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1187" spans="1:1">
       <c r="A1187">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1188" spans="1:1">
       <c r="A1188">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1189" spans="1:1">
       <c r="A1189">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1190" spans="1:1">
       <c r="A1190">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1191" spans="1:1">
       <c r="A1191">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1192" spans="1:1">
       <c r="A1192">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1193" spans="1:1">
       <c r="A1193">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1194" spans="1:1">
       <c r="A1194">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1195" spans="1:1">
       <c r="A1195">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1196" spans="1:1">
       <c r="A1196">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1197" spans="1:1">
       <c r="A1197">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1198" spans="1:1">
       <c r="A1198">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1199" spans="1:1">
       <c r="A1199">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1200" spans="1:1">
       <c r="A1200">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1201" spans="1:1">
       <c r="A1201">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1202" spans="1:1">
       <c r="A1202">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1203" spans="1:1">
       <c r="A1203">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1204" spans="1:1">
       <c r="A1204">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1205" spans="1:1">
       <c r="A1205">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1206" spans="1:1">
       <c r="A1206">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1207" spans="1:1">
       <c r="A1207">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1208" spans="1:1">
       <c r="A1208">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1209" spans="1:1">
       <c r="A1209">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1210" spans="1:1">
       <c r="A1210">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1211" spans="1:1">
       <c r="A1211">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1212" spans="1:1">
       <c r="A1212">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1213" spans="1:1">
       <c r="A1213">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1214" spans="1:1">
       <c r="A1214">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1215" spans="1:1">
       <c r="A1215">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1216" spans="1:1">
       <c r="A1216">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1217" spans="1:1">
       <c r="A1217">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1218" spans="1:1">
       <c r="A1218">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1219" spans="1:1">
       <c r="A1219">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1220" spans="1:1">
       <c r="A1220">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1221" spans="1:1">
       <c r="A1221">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1222" spans="1:1">
       <c r="A1222">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1223" spans="1:1">
       <c r="A1223">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1224" spans="1:1">
       <c r="A1224">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1225" spans="1:1">
       <c r="A1225">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1226" spans="1:1">
       <c r="A1226">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1227" spans="1:1">
       <c r="A1227">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1228" spans="1:1">
       <c r="A1228">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1229" spans="1:1">
       <c r="A1229">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1230" spans="1:1">
       <c r="A1230">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1231" spans="1:1">
       <c r="A1231">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1232" spans="1:1">
       <c r="A1232">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1233" spans="1:1">
       <c r="A1233">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1234" spans="1:1">
       <c r="A1234">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1235" spans="1:1">
       <c r="A1235">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1236" spans="1:1">
       <c r="A1236">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1237" spans="1:1">
       <c r="A1237">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1238" spans="1:1">
       <c r="A1238">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1239" spans="1:1">
       <c r="A1239">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1240" spans="1:1">
       <c r="A1240">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1241" spans="1:1">
       <c r="A1241">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1242" spans="1:1">
       <c r="A1242">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1243" spans="1:1">
       <c r="A1243">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1244" spans="1:1">
       <c r="A1244">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1245" spans="1:1">
       <c r="A1245">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1246" spans="1:1">
       <c r="A1246">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1247" spans="1:1">
       <c r="A1247">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1248" spans="1:1">
       <c r="A1248">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1249" spans="1:1">
       <c r="A1249">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1250" spans="1:1">
       <c r="A1250">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1251" spans="1:1">
       <c r="A1251">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1252" spans="1:1">
       <c r="A1252">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1253" spans="1:1">
       <c r="A1253">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1254" spans="1:1">
       <c r="A1254">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1255" spans="1:1">
       <c r="A1255">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1256" spans="1:1">
       <c r="A1256">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1257" spans="1:1">
       <c r="A1257">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1258" spans="1:1">
       <c r="A1258">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1259" spans="1:1">
       <c r="A1259">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1260" spans="1:1">
       <c r="A1260">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1261" spans="1:1">
       <c r="A1261">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1262" spans="1:1">
       <c r="A1262">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1263" spans="1:1">
       <c r="A1263">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1264" spans="1:1">
       <c r="A1264">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1265" spans="1:1">
       <c r="A1265">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1266" spans="1:1">
       <c r="A1266">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1267" spans="1:1">
       <c r="A1267">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1268" spans="1:1">
       <c r="A1268">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1269" spans="1:1">
       <c r="A1269">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1270" spans="1:1">
       <c r="A1270">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1271" spans="1:1">
       <c r="A1271">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1272" spans="1:1">
       <c r="A1272">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1273" spans="1:1">
       <c r="A1273">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1274" spans="1:1">
       <c r="A1274">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1275" spans="1:1">
       <c r="A1275">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1276" spans="1:1">
       <c r="A1276">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1277" spans="1:1">
       <c r="A1277">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1278" spans="1:1">
       <c r="A1278">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1279" spans="1:1">
       <c r="A1279">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1280" spans="1:1">
       <c r="A1280">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1281" spans="1:1">
       <c r="A1281">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1282" spans="1:1">
       <c r="A1282">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1283" spans="1:1">
       <c r="A1283">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1284" spans="1:1">
       <c r="A1284">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1285" spans="1:1">
       <c r="A1285">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1286" spans="1:1">
       <c r="A1286">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1287" spans="1:1">
       <c r="A1287">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1288" spans="1:1">
       <c r="A1288">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1289" spans="1:1">
       <c r="A1289">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1290" spans="1:1">
       <c r="A1290">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1291" spans="1:1">
       <c r="A1291">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1292" spans="1:1">
       <c r="A1292">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1293" spans="1:1">
       <c r="A1293">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1294" spans="1:1">
       <c r="A1294">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1295" spans="1:1">
       <c r="A1295">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1296" spans="1:1">
       <c r="A1296">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1297" spans="1:1">
       <c r="A1297">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1298" spans="1:1">
       <c r="A1298">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1299" spans="1:1">
       <c r="A1299">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1300" spans="1:1">
       <c r="A1300">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1301" spans="1:1">
       <c r="A1301">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1302" spans="1:1">
       <c r="A1302">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1303" spans="1:1">
       <c r="A1303">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1304" spans="1:1">
       <c r="A1304">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1305" spans="1:1">
       <c r="A1305">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1306" spans="1:1">
       <c r="A1306">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1307" spans="1:1">
       <c r="A1307">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1308" spans="1:1">
       <c r="A1308">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1309" spans="1:1">
       <c r="A1309">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1310" spans="1:1">
       <c r="A1310">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1311" spans="1:1">
       <c r="A1311">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1312" spans="1:1">
       <c r="A1312">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1313" spans="1:1">
       <c r="A1313">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1314" spans="1:1">
       <c r="A1314">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1315" spans="1:1">
       <c r="A1315">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1316" spans="1:1">
       <c r="A1316">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1317" spans="1:1">
       <c r="A1317">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1318" spans="1:1">
       <c r="A1318">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1319" spans="1:1">
       <c r="A1319">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1320" spans="1:1">
       <c r="A1320">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1321" spans="1:1">
       <c r="A1321">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1322" spans="1:1">
       <c r="A1322">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1323" spans="1:1">
       <c r="A1323">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1324" spans="1:1">
       <c r="A1324">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1325" spans="1:1">
       <c r="A1325">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1326" spans="1:1">
       <c r="A1326">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1327" spans="1:1">
       <c r="A1327">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1328" spans="1:1">
       <c r="A1328">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1329" spans="1:1">
       <c r="A1329">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1330" spans="1:1">
       <c r="A1330">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1331" spans="1:1">
       <c r="A1331">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1332" spans="1:1">
       <c r="A1332">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1333" spans="1:1">
       <c r="A1333">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1334" spans="1:1">
       <c r="A1334">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1335" spans="1:1">
       <c r="A1335">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1336" spans="1:1">
       <c r="A1336">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1337" spans="1:1">
       <c r="A1337">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1338" spans="1:1">
       <c r="A1338">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1339" spans="1:1">
       <c r="A1339">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1340" spans="1:1">
       <c r="A1340">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1341" spans="1:1">
       <c r="A1341">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1342" spans="1:1">
@@ -11279,202 +11279,202 @@
     </row>
     <row r="2182" spans="1:1">
       <c r="A2182">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2183" spans="1:1">
       <c r="A2183">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2184" spans="1:1">
       <c r="A2184">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2185" spans="1:1">
       <c r="A2185">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2186" spans="1:1">
       <c r="A2186">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2187" spans="1:1">
       <c r="A2187">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2188" spans="1:1">
       <c r="A2188">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2189" spans="1:1">
       <c r="A2189">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2190" spans="1:1">
       <c r="A2190">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2191" spans="1:1">
       <c r="A2191">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2192" spans="1:1">
       <c r="A2192">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2193" spans="1:1">
       <c r="A2193">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2194" spans="1:1">
       <c r="A2194">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2195" spans="1:1">
       <c r="A2195">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2196" spans="1:1">
       <c r="A2196">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2197" spans="1:1">
       <c r="A2197">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2198" spans="1:1">
       <c r="A2198">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2199" spans="1:1">
       <c r="A2199">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2200" spans="1:1">
       <c r="A2200">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2201" spans="1:1">
       <c r="A2201">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2202" spans="1:1">
       <c r="A2202">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2203" spans="1:1">
       <c r="A2203">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2204" spans="1:1">
       <c r="A2204">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2205" spans="1:1">
       <c r="A2205">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2206" spans="1:1">
       <c r="A2206">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2207" spans="1:1">
       <c r="A2207">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2208" spans="1:1">
       <c r="A2208">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2209" spans="1:1">
       <c r="A2209">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2210" spans="1:1">
       <c r="A2210">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2211" spans="1:1">
       <c r="A2211">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2212" spans="1:1">
       <c r="A2212">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2213" spans="1:1">
       <c r="A2213">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2214" spans="1:1">
       <c r="A2214">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2215" spans="1:1">
       <c r="A2215">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2216" spans="1:1">
       <c r="A2216">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2217" spans="1:1">
       <c r="A2217">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2218" spans="1:1">
       <c r="A2218">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2219" spans="1:1">
       <c r="A2219">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2220" spans="1:1">
       <c r="A2220">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2221" spans="1:1">
       <c r="A2221">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2222" spans="1:1">
@@ -11629,292 +11629,292 @@
     </row>
     <row r="2252" spans="1:1">
       <c r="A2252">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2253" spans="1:1">
       <c r="A2253">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2254" spans="1:1">
       <c r="A2254">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2255" spans="1:1">
       <c r="A2255">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2256" spans="1:1">
       <c r="A2256">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2257" spans="1:1">
       <c r="A2257">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2258" spans="1:1">
       <c r="A2258">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2259" spans="1:1">
       <c r="A2259">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2260" spans="1:1">
       <c r="A2260">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2261" spans="1:1">
       <c r="A2261">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2262" spans="1:1">
       <c r="A2262">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2263" spans="1:1">
       <c r="A2263">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2264" spans="1:1">
       <c r="A2264">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2265" spans="1:1">
       <c r="A2265">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2266" spans="1:1">
       <c r="A2266">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2267" spans="1:1">
       <c r="A2267">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2268" spans="1:1">
       <c r="A2268">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2269" spans="1:1">
       <c r="A2269">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2270" spans="1:1">
       <c r="A2270">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2271" spans="1:1">
       <c r="A2271">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2272" spans="1:1">
       <c r="A2272">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2273" spans="1:1">
       <c r="A2273">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2274" spans="1:1">
       <c r="A2274">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2275" spans="1:1">
       <c r="A2275">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2276" spans="1:1">
       <c r="A2276">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2277" spans="1:1">
       <c r="A2277">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2278" spans="1:1">
       <c r="A2278">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2279" spans="1:1">
       <c r="A2279">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2280" spans="1:1">
       <c r="A2280">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2281" spans="1:1">
       <c r="A2281">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2282" spans="1:1">
       <c r="A2282">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2283" spans="1:1">
       <c r="A2283">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2284" spans="1:1">
       <c r="A2284">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2285" spans="1:1">
       <c r="A2285">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2286" spans="1:1">
       <c r="A2286">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2287" spans="1:1">
       <c r="A2287">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2288" spans="1:1">
       <c r="A2288">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2289" spans="1:1">
       <c r="A2289">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2290" spans="1:1">
       <c r="A2290">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2291" spans="1:1">
       <c r="A2291">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2292" spans="1:1">
       <c r="A2292">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2293" spans="1:1">
       <c r="A2293">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2294" spans="1:1">
       <c r="A2294">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2295" spans="1:1">
       <c r="A2295">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2296" spans="1:1">
       <c r="A2296">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2297" spans="1:1">
       <c r="A2297">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2298" spans="1:1">
       <c r="A2298">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2299" spans="1:1">
       <c r="A2299">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2300" spans="1:1">
       <c r="A2300">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2301" spans="1:1">
       <c r="A2301">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2302" spans="1:1">
       <c r="A2302">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2303" spans="1:1">
       <c r="A2303">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2304" spans="1:1">
       <c r="A2304">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2305" spans="1:1">
       <c r="A2305">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2306" spans="1:1">
       <c r="A2306">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2307" spans="1:1">
       <c r="A2307">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2308" spans="1:1">
       <c r="A2308">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2309" spans="1:1">
       <c r="A2309">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2310" spans="1:1">
@@ -12779,172 +12779,172 @@
     </row>
     <row r="2482" spans="1:1">
       <c r="A2482">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2483" spans="1:1">
       <c r="A2483">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2484" spans="1:1">
       <c r="A2484">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2485" spans="1:1">
       <c r="A2485">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2486" spans="1:1">
       <c r="A2486">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2487" spans="1:1">
       <c r="A2487">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2488" spans="1:1">
       <c r="A2488">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2489" spans="1:1">
       <c r="A2489">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2490" spans="1:1">
       <c r="A2490">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2491" spans="1:1">
       <c r="A2491">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2492" spans="1:1">
       <c r="A2492">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2493" spans="1:1">
       <c r="A2493">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2494" spans="1:1">
       <c r="A2494">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2495" spans="1:1">
       <c r="A2495">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2496" spans="1:1">
       <c r="A2496">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2497" spans="1:1">
       <c r="A2497">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2498" spans="1:1">
       <c r="A2498">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2499" spans="1:1">
       <c r="A2499">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2500" spans="1:1">
       <c r="A2500">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2501" spans="1:1">
       <c r="A2501">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2502" spans="1:1">
       <c r="A2502">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2503" spans="1:1">
       <c r="A2503">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2504" spans="1:1">
       <c r="A2504">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2505" spans="1:1">
       <c r="A2505">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2506" spans="1:1">
       <c r="A2506">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2507" spans="1:1">
       <c r="A2507">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2508" spans="1:1">
       <c r="A2508">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2509" spans="1:1">
       <c r="A2509">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2510" spans="1:1">
       <c r="A2510">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2511" spans="1:1">
       <c r="A2511">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2512" spans="1:1">
       <c r="A2512">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2513" spans="1:1">
       <c r="A2513">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2514" spans="1:1">
       <c r="A2514">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2515" spans="1:1">
       <c r="A2515">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2516" spans="1:1">
@@ -14029,52 +14029,52 @@
     </row>
     <row r="2732" spans="1:1">
       <c r="A2732">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2733" spans="1:1">
       <c r="A2733">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2734" spans="1:1">
       <c r="A2734">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2735" spans="1:1">
       <c r="A2735">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2736" spans="1:1">
       <c r="A2736">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2737" spans="1:1">
       <c r="A2737">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2738" spans="1:1">
       <c r="A2738">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2739" spans="1:1">
       <c r="A2739">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2740" spans="1:1">
       <c r="A2740">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2741" spans="1:1">
       <c r="A2741">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2742" spans="1:1">
@@ -14364,417 +14364,417 @@
     </row>
     <row r="2799" spans="1:1">
       <c r="A2799">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2800" spans="1:1">
       <c r="A2800">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2801" spans="1:1">
       <c r="A2801">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2802" spans="1:1">
       <c r="A2802">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2803" spans="1:1">
       <c r="A2803">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2804" spans="1:1">
       <c r="A2804">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2805" spans="1:1">
       <c r="A2805">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2806" spans="1:1">
       <c r="A2806">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2807" spans="1:1">
       <c r="A2807">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2808" spans="1:1">
       <c r="A2808">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2809" spans="1:1">
       <c r="A2809">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2810" spans="1:1">
       <c r="A2810">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2811" spans="1:1">
       <c r="A2811">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2812" spans="1:1">
       <c r="A2812">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2813" spans="1:1">
       <c r="A2813">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2814" spans="1:1">
       <c r="A2814">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2815" spans="1:1">
       <c r="A2815">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2816" spans="1:1">
       <c r="A2816">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2817" spans="1:1">
       <c r="A2817">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2818" spans="1:1">
       <c r="A2818">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2819" spans="1:1">
       <c r="A2819">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2820" spans="1:1">
       <c r="A2820">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2821" spans="1:1">
       <c r="A2821">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2822" spans="1:1">
       <c r="A2822">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2823" spans="1:1">
       <c r="A2823">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2824" spans="1:1">
       <c r="A2824">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2825" spans="1:1">
       <c r="A2825">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2826" spans="1:1">
       <c r="A2826">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2827" spans="1:1">
       <c r="A2827">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2828" spans="1:1">
       <c r="A2828">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2829" spans="1:1">
       <c r="A2829">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2830" spans="1:1">
       <c r="A2830">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2831" spans="1:1">
       <c r="A2831">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2832" spans="1:1">
       <c r="A2832">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2833" spans="1:1">
       <c r="A2833">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2834" spans="1:1">
       <c r="A2834">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2835" spans="1:1">
       <c r="A2835">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2836" spans="1:1">
       <c r="A2836">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2837" spans="1:1">
       <c r="A2837">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2838" spans="1:1">
       <c r="A2838">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2839" spans="1:1">
       <c r="A2839">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2840" spans="1:1">
       <c r="A2840">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2841" spans="1:1">
       <c r="A2841">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2842" spans="1:1">
       <c r="A2842">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2843" spans="1:1">
       <c r="A2843">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2844" spans="1:1">
       <c r="A2844">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2845" spans="1:1">
       <c r="A2845">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2846" spans="1:1">
       <c r="A2846">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2847" spans="1:1">
       <c r="A2847">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2848" spans="1:1">
       <c r="A2848">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2849" spans="1:1">
       <c r="A2849">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2850" spans="1:1">
       <c r="A2850">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2851" spans="1:1">
       <c r="A2851">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2852" spans="1:1">
       <c r="A2852">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2853" spans="1:1">
       <c r="A2853">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2854" spans="1:1">
       <c r="A2854">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2855" spans="1:1">
       <c r="A2855">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2856" spans="1:1">
       <c r="A2856">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2857" spans="1:1">
       <c r="A2857">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2858" spans="1:1">
       <c r="A2858">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2859" spans="1:1">
       <c r="A2859">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2860" spans="1:1">
       <c r="A2860">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2861" spans="1:1">
       <c r="A2861">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2862" spans="1:1">
       <c r="A2862">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2863" spans="1:1">
       <c r="A2863">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2864" spans="1:1">
       <c r="A2864">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2865" spans="1:1">
       <c r="A2865">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2866" spans="1:1">
       <c r="A2866">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2867" spans="1:1">
       <c r="A2867">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2868" spans="1:1">
       <c r="A2868">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2869" spans="1:1">
       <c r="A2869">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2870" spans="1:1">
       <c r="A2870">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2871" spans="1:1">
       <c r="A2871">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2872" spans="1:1">
       <c r="A2872">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2873" spans="1:1">
       <c r="A2873">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2874" spans="1:1">
       <c r="A2874">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2875" spans="1:1">
       <c r="A2875">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2876" spans="1:1">
       <c r="A2876">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2877" spans="1:1">
       <c r="A2877">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2878" spans="1:1">
       <c r="A2878">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2879" spans="1:1">
       <c r="A2879">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2880" spans="1:1">
       <c r="A2880">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="2881" spans="1:1">
       <c r="A2881">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>